<commit_message>
Añadido visor control. Más fácil depurar ahora.
</commit_message>
<xml_diff>
--- a/resources/calculaCoordenadas.xlsx
+++ b/resources/calculaCoordenadas.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Universidad de Málaga\proyectos\riscv\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uma365-my.sharepoint.com/personal/felipe_uma_es/Documents/proyectos/riscv/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A892972-94E9-4781-A28B-04457C923476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{616F939D-A7BF-44E5-BB31-AF8BDBB5B329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BDCD06E-1755-4FB5-A6DF-1ED26566B674}"/>
+    <workbookView xWindow="6510" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{8BDCD06E-1755-4FB5-A6DF-1ED26566B674}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,12 +30,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Calculadora de coordenadas relativas</t>
   </si>
@@ -61,6 +65,18 @@
   </si>
   <si>
     <t>Registros pipeline</t>
+  </si>
+  <si>
+    <t>Banco de registros</t>
+  </si>
+  <si>
+    <t>Derecho Buffer Instr</t>
+  </si>
+  <si>
+    <t>NPCs</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -412,38 +428,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B07CB80-7603-4E63-B9E3-E01CF302815B}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
         <v>160</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
       </c>
       <c r="F6">
         <v>230</v>
@@ -453,21 +469,29 @@
         <v>0.26923076923076922</v>
       </c>
       <c r="I6">
-        <v>242</v>
+        <f>G25</f>
+        <v>224</v>
       </c>
       <c r="J6">
         <f>(I6-$B$6)/$B$8</f>
+        <v>0.24615384615384617</v>
+      </c>
+      <c r="K6">
+        <v>242</v>
+      </c>
+      <c r="L6">
+        <f>(K6-$B$6)/$B$8</f>
         <v>0.31538461538461537</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>190</v>
       </c>
-      <c r="N6">
-        <f>(M6-$B$6)/$B$8</f>
+      <c r="P6">
+        <f>(O6-$B$6)/$B$8</f>
         <v>0.11538461538461539</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -482,21 +506,29 @@
         <v>0.45384615384615384</v>
       </c>
       <c r="I7">
-        <v>260</v>
+        <f>G26</f>
+        <v>248</v>
       </c>
       <c r="J7">
         <f>(I7-$B$6)/$B$8</f>
+        <v>0.33846153846153848</v>
+      </c>
+      <c r="K7">
+        <v>260</v>
+      </c>
+      <c r="L7">
+        <f>(K7-$B$6)/$B$8</f>
         <v>0.38461538461538464</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>270</v>
       </c>
-      <c r="N7">
-        <f>(M7-$B$6)/$B$8</f>
+      <c r="P7">
+        <f>(O7-$B$6)/$B$8</f>
         <v>0.42307692307692307</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -512,21 +544,29 @@
         <v>0.71153846153846156</v>
       </c>
       <c r="I8">
-        <v>330</v>
+        <f>G27</f>
+        <v>272</v>
       </c>
       <c r="J8">
         <f>(I8-$B$6)/$B$8</f>
+        <v>0.43076923076923079</v>
+      </c>
+      <c r="K8">
+        <v>330</v>
+      </c>
+      <c r="L8">
+        <f>(K8-$B$6)/$B$8</f>
         <v>0.65384615384615385</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>345</v>
       </c>
-      <c r="N8">
-        <f>(M8-$B$6)/$B$8</f>
+      <c r="P8">
+        <f>(O8-$B$6)/$B$8</f>
         <v>0.71153846153846156</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>380</v>
       </c>
@@ -535,58 +575,248 @@
         <v>0.84615384615384615</v>
       </c>
       <c r="I9">
-        <v>345</v>
+        <f>G28</f>
+        <v>296</v>
       </c>
       <c r="J9">
         <f>(I9-$B$6)/$B$8</f>
+        <v>0.52307692307692311</v>
+      </c>
+      <c r="K9">
+        <v>345</v>
+      </c>
+      <c r="L9">
+        <f>(K9-$B$6)/$B$8</f>
         <v>0.71153846153846156</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
+      <c r="B18">
         <v>200</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E18" t="s">
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="F18">
         <v>0.25</v>
       </c>
-      <c r="G12">
-        <f>$B$12+F12*$B$14</f>
+      <c r="G18">
+        <f>$B$18+F18*$B$20</f>
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B13">
+      <c r="B19">
         <v>320</v>
       </c>
-      <c r="F13">
+      <c r="F19">
         <v>0.65</v>
       </c>
-      <c r="G13">
-        <f>$B$12+F13*$B$14</f>
+      <c r="G19">
+        <f>$B$18+F19*$B$20</f>
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B14">
-        <f>B13-B12</f>
+      <c r="B20">
+        <f>B19-B18</f>
         <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>0.2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:G30" si="0">$B$18+F25*$B$20</f>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>220</v>
+      </c>
+      <c r="F26">
+        <v>0.4</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>B26-B25</f>
+        <v>120</v>
+      </c>
+      <c r="F27">
+        <v>0.6</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>0.8</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>0.25</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>0.65</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>120</v>
+      </c>
+      <c r="F32">
+        <v>150</v>
+      </c>
+      <c r="G32">
+        <f>(F32-$B$32)/$B$34</f>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>275</v>
+      </c>
+      <c r="F37">
+        <v>480</v>
+      </c>
+      <c r="G37">
+        <f>(F37-$B$37)/$B$39</f>
+        <v>0.19158878504672897</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>560</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G45" si="1">(F38-$B$37)/$B$39</f>
+        <v>0.26635514018691586</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1070</v>
+      </c>
+      <c r="F39">
+        <v>615</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>0.31775700934579437</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>660</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>0.35981308411214952</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>870</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>0.55607476635514019</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>950</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>0.63084112149532712</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>1050</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>0.72429906542056077</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>1140</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>0.80841121495327106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>1316.66</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>0.97351401869158882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ventana de instrucciones, Unidades hazards
</commit_message>
<xml_diff>
--- a/resources/calculaCoordenadas.xlsx
+++ b/resources/calculaCoordenadas.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uma365-my.sharepoint.com/personal/felipe_uma_es/Documents/proyectos/riscv/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{616F939D-A7BF-44E5-BB31-AF8BDBB5B329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{616F939D-A7BF-44E5-BB31-AF8BDBB5B329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC2EC123-6B2A-4045-8D23-3CCDCF2E93AA}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{8BDCD06E-1755-4FB5-A6DF-1ED26566B674}"/>
+    <workbookView xWindow="24630" yWindow="2865" windowWidth="18900" windowHeight="10965" xr2:uid="{8BDCD06E-1755-4FB5-A6DF-1ED26566B674}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B07CB80-7603-4E63-B9E3-E01CF302815B}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37:G45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,11 +775,11 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F41">
-        <v>870</v>
+        <v>820</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>0.55607476635514019</v>
+        <v>0.50934579439252337</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,11 +811,11 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F45">
-        <v>1316.66</v>
+        <v>1296</v>
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
-        <v>0.97351401869158882</v>
+        <v>0.95420560747663552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>